<commit_message>
adding markers to 920 903 hbrown
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_08.20.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_08.20.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="62">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">replicate</t>
   </si>
   <si>
+    <t xml:space="preserve">marker_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">08.20.20</t>
   </si>
   <si>
@@ -73,10 +76,16 @@
     <t xml:space="preserve">CNAG_03018</t>
   </si>
   <si>
+    <t xml:space="preserve">G418</t>
+  </si>
+  <si>
     <t xml:space="preserve">TDY1326</t>
   </si>
   <si>
     <t xml:space="preserve">CNAG_03279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAT</t>
   </si>
   <si>
     <t xml:space="preserve">TDY1335</t>
@@ -294,10 +303,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -335,28 +344,31 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>90</v>
@@ -367,25 +379,25 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>90</v>
@@ -396,344 +408,377 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>90</v>
@@ -744,199 +789,217 @@
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>21</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>90</v>
@@ -947,25 +1010,25 @@
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>22</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>90</v>
@@ -976,25 +1039,25 @@
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>23</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>90</v>
@@ -1005,31 +1068,34 @@
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>24</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>90</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>